<commit_message>
Joint all dataset in Problem 3
</commit_message>
<xml_diff>
--- a/data/Trash-Wheel-Collection-Totals-7-2020-2.xlsx
+++ b/data/Trash-Wheel-Collection-Totals-7-2020-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mengxisun/Documents/Fall 2022/Data Science I/p8105_hw2_ms6360/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8938430-D5AF-1F40-A9B1-2605BD74CB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525476E8-85FC-F84F-9BEB-D2331C7349BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="15820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Homes powered note" sheetId="5" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mr. Trash Wheel'!$A$1:$O$294</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mr. Trash Wheel'!$A$2:$O$534</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1374,12 +1374,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,6 +1407,12 @@
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2415,10 +2415,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DL547"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A501" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="M475" sqref="M475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -2439,20 +2439,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="203"/>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
+      <c r="A1" s="218"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+      <c r="L1" s="218"/>
+      <c r="M1" s="218"/>
+      <c r="N1" s="218"/>
     </row>
     <row r="2" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -2491,7 +2491,7 @@
       <c r="L2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="205" t="s">
+      <c r="M2" s="203" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="13" t="s">
@@ -16866,7 +16866,7 @@
         <f t="shared" si="60"/>
         <v>19360</v>
       </c>
-      <c r="M312" s="206">
+      <c r="M312" s="204">
         <f t="shared" si="60"/>
         <v>27</v>
       </c>
@@ -21625,7 +21625,7 @@
       <c r="L408" s="33">
         <v>1380</v>
       </c>
-      <c r="M408" s="207">
+      <c r="M408" s="205">
         <v>11</v>
       </c>
       <c r="N408" s="22">
@@ -21671,7 +21671,7 @@
       <c r="L409" s="33">
         <v>1500</v>
       </c>
-      <c r="M409" s="207">
+      <c r="M409" s="205">
         <v>8</v>
       </c>
       <c r="N409" s="22">
@@ -21717,7 +21717,7 @@
       <c r="L410" s="33">
         <v>980</v>
       </c>
-      <c r="M410" s="207">
+      <c r="M410" s="205">
         <v>20</v>
       </c>
       <c r="N410" s="22">
@@ -21763,7 +21763,7 @@
       <c r="L411" s="33">
         <v>680</v>
       </c>
-      <c r="M411" s="207">
+      <c r="M411" s="205">
         <v>7</v>
       </c>
       <c r="N411" s="22">
@@ -21809,7 +21809,7 @@
       <c r="L412" s="33">
         <v>1100</v>
       </c>
-      <c r="M412" s="207">
+      <c r="M412" s="205">
         <v>8</v>
       </c>
       <c r="N412" s="22">
@@ -21855,7 +21855,7 @@
       <c r="L413" s="33">
         <v>1400</v>
       </c>
-      <c r="M413" s="207">
+      <c r="M413" s="205">
         <v>18</v>
       </c>
       <c r="N413" s="22">
@@ -21901,7 +21901,7 @@
       <c r="L414" s="33">
         <v>1440</v>
       </c>
-      <c r="M414" s="207">
+      <c r="M414" s="205">
         <v>14</v>
       </c>
       <c r="N414" s="22">
@@ -21947,7 +21947,7 @@
       <c r="L415" s="33">
         <v>2040</v>
       </c>
-      <c r="M415" s="207">
+      <c r="M415" s="205">
         <v>22</v>
       </c>
       <c r="N415" s="22">
@@ -21993,7 +21993,7 @@
       <c r="L416" s="33">
         <v>1340</v>
       </c>
-      <c r="M416" s="207">
+      <c r="M416" s="205">
         <v>12</v>
       </c>
       <c r="N416" s="22">
@@ -22039,7 +22039,7 @@
       <c r="L417" s="33">
         <v>740</v>
       </c>
-      <c r="M417" s="207">
+      <c r="M417" s="205">
         <v>4</v>
       </c>
       <c r="N417" s="22">
@@ -22085,7 +22085,7 @@
       <c r="L418" s="33">
         <v>1800</v>
       </c>
-      <c r="M418" s="207">
+      <c r="M418" s="205">
         <v>14</v>
       </c>
       <c r="N418" s="22">
@@ -22131,7 +22131,7 @@
       <c r="L419" s="33">
         <v>1600</v>
       </c>
-      <c r="M419" s="207">
+      <c r="M419" s="205">
         <v>32</v>
       </c>
       <c r="N419" s="22">
@@ -22226,7 +22226,7 @@
       <c r="L421" s="33">
         <v>1380</v>
       </c>
-      <c r="M421" s="207">
+      <c r="M421" s="205">
         <v>10</v>
       </c>
       <c r="N421" s="22">
@@ -22272,7 +22272,7 @@
       <c r="L422" s="33">
         <v>640</v>
       </c>
-      <c r="M422" s="207">
+      <c r="M422" s="205">
         <v>4</v>
       </c>
       <c r="N422" s="22">
@@ -22318,7 +22318,7 @@
       <c r="L423" s="33">
         <v>1310</v>
       </c>
-      <c r="M423" s="207">
+      <c r="M423" s="205">
         <v>14</v>
       </c>
       <c r="N423" s="22">
@@ -22364,7 +22364,7 @@
       <c r="L424" s="33">
         <v>240</v>
       </c>
-      <c r="M424" s="207">
+      <c r="M424" s="205">
         <v>0</v>
       </c>
       <c r="N424" s="22">
@@ -22410,7 +22410,7 @@
       <c r="L425" s="33">
         <v>540</v>
       </c>
-      <c r="M425" s="207">
+      <c r="M425" s="205">
         <v>6</v>
       </c>
       <c r="N425" s="22">
@@ -22456,7 +22456,7 @@
       <c r="L426" s="33">
         <v>980</v>
       </c>
-      <c r="M426" s="207">
+      <c r="M426" s="205">
         <v>13</v>
       </c>
       <c r="N426" s="22">
@@ -22502,7 +22502,7 @@
       <c r="L427" s="33">
         <v>960</v>
       </c>
-      <c r="M427" s="207">
+      <c r="M427" s="205">
         <v>21</v>
       </c>
       <c r="N427" s="22">
@@ -22597,7 +22597,7 @@
       <c r="L429" s="86">
         <v>1100</v>
       </c>
-      <c r="M429" s="208">
+      <c r="M429" s="206">
         <v>4</v>
       </c>
       <c r="N429" s="22">
@@ -22643,7 +22643,7 @@
       <c r="L430" s="86">
         <v>1200</v>
       </c>
-      <c r="M430" s="208">
+      <c r="M430" s="206">
         <v>12</v>
       </c>
       <c r="N430" s="22">
@@ -22689,7 +22689,7 @@
       <c r="L431" s="86">
         <v>2100</v>
       </c>
-      <c r="M431" s="208">
+      <c r="M431" s="206">
         <v>16</v>
       </c>
       <c r="N431" s="22">
@@ -22735,7 +22735,7 @@
       <c r="L432" s="86">
         <v>1980</v>
       </c>
-      <c r="M432" s="208">
+      <c r="M432" s="206">
         <v>28</v>
       </c>
       <c r="N432" s="22">
@@ -22781,7 +22781,7 @@
       <c r="L433" s="86">
         <v>1400</v>
       </c>
-      <c r="M433" s="208">
+      <c r="M433" s="206">
         <v>12</v>
       </c>
       <c r="N433" s="22">
@@ -22827,7 +22827,7 @@
       <c r="L434" s="86">
         <v>1580</v>
       </c>
-      <c r="M434" s="208">
+      <c r="M434" s="206">
         <v>20</v>
       </c>
       <c r="N434" s="22">
@@ -22873,7 +22873,7 @@
       <c r="L435" s="86">
         <v>560</v>
       </c>
-      <c r="M435" s="208">
+      <c r="M435" s="206">
         <v>4</v>
       </c>
       <c r="N435" s="22">
@@ -22919,7 +22919,7 @@
       <c r="L436" s="86">
         <v>880</v>
       </c>
-      <c r="M436" s="208">
+      <c r="M436" s="206">
         <v>2</v>
       </c>
       <c r="N436" s="22">
@@ -22967,7 +22967,7 @@
         <f t="shared" si="82"/>
         <v>10800</v>
       </c>
-      <c r="M437" s="209">
+      <c r="M437" s="207">
         <f t="shared" si="82"/>
         <v>98</v>
       </c>
@@ -23014,7 +23014,7 @@
       <c r="L438" s="86">
         <v>560</v>
       </c>
-      <c r="M438" s="208">
+      <c r="M438" s="206">
         <v>12</v>
       </c>
       <c r="N438" s="22">
@@ -23060,7 +23060,7 @@
       <c r="L439" s="86">
         <v>880</v>
       </c>
-      <c r="M439" s="208">
+      <c r="M439" s="206">
         <v>2</v>
       </c>
       <c r="N439" s="22">
@@ -23106,7 +23106,7 @@
       <c r="L440" s="86">
         <v>1020</v>
       </c>
-      <c r="M440" s="208">
+      <c r="M440" s="206">
         <v>11</v>
       </c>
       <c r="N440" s="22">
@@ -23152,7 +23152,7 @@
       <c r="L441" s="86">
         <v>400</v>
       </c>
-      <c r="M441" s="208">
+      <c r="M441" s="206">
         <v>4</v>
       </c>
       <c r="N441" s="22">
@@ -23198,7 +23198,7 @@
       <c r="L442" s="86">
         <v>720</v>
       </c>
-      <c r="M442" s="208">
+      <c r="M442" s="206">
         <v>1</v>
       </c>
       <c r="N442" s="22">
@@ -23244,7 +23244,7 @@
       <c r="L443" s="86">
         <v>190</v>
       </c>
-      <c r="M443" s="208">
+      <c r="M443" s="206">
         <v>0</v>
       </c>
       <c r="N443" s="22">
@@ -23290,7 +23290,7 @@
       <c r="L444" s="86">
         <v>240</v>
       </c>
-      <c r="M444" s="208">
+      <c r="M444" s="206">
         <v>3</v>
       </c>
       <c r="N444" s="22">
@@ -23338,7 +23338,7 @@
         <f t="shared" si="83"/>
         <v>4010</v>
       </c>
-      <c r="M445" s="209">
+      <c r="M445" s="207">
         <f t="shared" si="83"/>
         <v>33</v>
       </c>
@@ -23385,7 +23385,7 @@
       <c r="L446" s="86">
         <v>1200</v>
       </c>
-      <c r="M446" s="208">
+      <c r="M446" s="206">
         <v>9</v>
       </c>
       <c r="N446" s="22">
@@ -23431,7 +23431,7 @@
       <c r="L447" s="86">
         <v>1700</v>
       </c>
-      <c r="M447" s="208">
+      <c r="M447" s="206">
         <v>12</v>
       </c>
       <c r="N447" s="22">
@@ -23479,7 +23479,7 @@
         <f t="shared" si="84"/>
         <v>2900</v>
       </c>
-      <c r="M448" s="209">
+      <c r="M448" s="207">
         <f t="shared" si="84"/>
         <v>21</v>
       </c>
@@ -23526,7 +23526,7 @@
       <c r="L449" s="97">
         <v>1100</v>
       </c>
-      <c r="M449" s="210">
+      <c r="M449" s="208">
         <v>16</v>
       </c>
       <c r="N449" s="22">
@@ -23571,7 +23571,7 @@
       <c r="L450" s="97">
         <v>1800</v>
       </c>
-      <c r="M450" s="210">
+      <c r="M450" s="208">
         <v>12</v>
       </c>
       <c r="N450" s="22">
@@ -23616,7 +23616,7 @@
       <c r="L451" s="97">
         <v>980</v>
       </c>
-      <c r="M451" s="210">
+      <c r="M451" s="208">
         <v>8</v>
       </c>
       <c r="N451" s="22">
@@ -23661,7 +23661,7 @@
       <c r="L452" s="97">
         <v>1450</v>
       </c>
-      <c r="M452" s="210">
+      <c r="M452" s="208">
         <v>6</v>
       </c>
       <c r="N452" s="22">
@@ -23706,7 +23706,7 @@
       <c r="L453" s="97">
         <v>840</v>
       </c>
-      <c r="M453" s="210">
+      <c r="M453" s="208">
         <v>14</v>
       </c>
       <c r="N453" s="22">
@@ -23751,7 +23751,7 @@
       <c r="L454" s="97">
         <v>640</v>
       </c>
-      <c r="M454" s="210">
+      <c r="M454" s="208">
         <v>2</v>
       </c>
       <c r="N454" s="22">
@@ -23796,7 +23796,7 @@
       <c r="L455" s="97">
         <v>560</v>
       </c>
-      <c r="M455" s="210">
+      <c r="M455" s="208">
         <v>6</v>
       </c>
       <c r="N455" s="22">
@@ -23841,7 +23841,7 @@
       <c r="L456" s="97">
         <v>1200</v>
       </c>
-      <c r="M456" s="210">
+      <c r="M456" s="208">
         <v>14</v>
       </c>
       <c r="N456" s="22">
@@ -23886,7 +23886,7 @@
       <c r="L457" s="97">
         <v>980</v>
       </c>
-      <c r="M457" s="210">
+      <c r="M457" s="208">
         <v>10</v>
       </c>
       <c r="N457" s="22">
@@ -23933,7 +23933,7 @@
         <f t="shared" si="85"/>
         <v>9550</v>
       </c>
-      <c r="M458" s="211">
+      <c r="M458" s="209">
         <f t="shared" si="85"/>
         <v>88</v>
       </c>
@@ -23980,7 +23980,7 @@
       <c r="L459" s="97">
         <v>1040</v>
       </c>
-      <c r="M459" s="210">
+      <c r="M459" s="208">
         <v>9</v>
       </c>
       <c r="N459" s="22">
@@ -24027,7 +24027,7 @@
         <f t="shared" si="86"/>
         <v>1040</v>
       </c>
-      <c r="M460" s="211">
+      <c r="M460" s="209">
         <f t="shared" si="86"/>
         <v>9</v>
       </c>
@@ -24074,7 +24074,7 @@
       <c r="L461" s="97">
         <v>800</v>
       </c>
-      <c r="M461" s="210">
+      <c r="M461" s="208">
         <v>16</v>
       </c>
       <c r="N461" s="22">
@@ -24119,7 +24119,7 @@
       <c r="L462" s="97">
         <v>1000</v>
       </c>
-      <c r="M462" s="210">
+      <c r="M462" s="208">
         <v>7</v>
       </c>
       <c r="N462" s="22">
@@ -24164,7 +24164,7 @@
       <c r="L463" s="97">
         <v>1040</v>
       </c>
-      <c r="M463" s="210">
+      <c r="M463" s="208">
         <v>11</v>
       </c>
       <c r="N463" s="22">
@@ -24211,7 +24211,7 @@
         <f t="shared" si="87"/>
         <v>2840</v>
       </c>
-      <c r="M464" s="211">
+      <c r="M464" s="209">
         <f t="shared" si="87"/>
         <v>34</v>
       </c>
@@ -24221,7 +24221,7 @@
       </c>
       <c r="O464" s="96"/>
     </row>
-    <row r="465" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A465" s="97">
         <v>394</v>
       </c>
@@ -24258,7 +24258,7 @@
       <c r="L465" s="97">
         <v>1640</v>
       </c>
-      <c r="M465" s="210">
+      <c r="M465" s="208">
         <v>6</v>
       </c>
       <c r="N465" s="22">
@@ -24266,7 +24266,7 @@
         <v>66.333333333333329</v>
       </c>
     </row>
-    <row r="466" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A466" s="97">
         <v>395</v>
       </c>
@@ -24303,7 +24303,7 @@
       <c r="L466" s="97">
         <v>1200</v>
       </c>
-      <c r="M466" s="210">
+      <c r="M466" s="208">
         <v>14</v>
       </c>
       <c r="N466" s="22">
@@ -24311,7 +24311,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="467" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A467" s="97">
         <v>396</v>
       </c>
@@ -24348,7 +24348,7 @@
       <c r="L467" s="97">
         <v>800</v>
       </c>
-      <c r="M467" s="210">
+      <c r="M467" s="208">
         <v>8</v>
       </c>
       <c r="N467" s="22">
@@ -24356,7 +24356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="468" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A468" s="97">
         <v>397</v>
       </c>
@@ -24393,7 +24393,7 @@
       <c r="L468" s="97">
         <v>380</v>
       </c>
-      <c r="M468" s="210">
+      <c r="M468" s="208">
         <v>4</v>
       </c>
       <c r="N468" s="22">
@@ -24401,7 +24401,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="469" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A469" s="97">
         <v>398</v>
       </c>
@@ -24438,7 +24438,7 @@
       <c r="L469" s="97">
         <v>340</v>
       </c>
-      <c r="M469" s="210">
+      <c r="M469" s="208">
         <v>4</v>
       </c>
       <c r="N469" s="22">
@@ -24446,7 +24446,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="470" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A470" s="97">
         <v>399</v>
       </c>
@@ -24483,7 +24483,7 @@
       <c r="L470" s="97">
         <v>290</v>
       </c>
-      <c r="M470" s="210">
+      <c r="M470" s="208">
         <v>2</v>
       </c>
       <c r="N470" s="22">
@@ -24491,7 +24491,7 @@
         <v>52.166666666666664</v>
       </c>
     </row>
-    <row r="471" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A471" s="97">
         <v>400</v>
       </c>
@@ -24528,7 +24528,7 @@
       <c r="L471" s="97">
         <v>1600</v>
       </c>
-      <c r="M471" s="210">
+      <c r="M471" s="208">
         <v>14</v>
       </c>
       <c r="N471" s="22">
@@ -24536,7 +24536,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="472" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A472" s="97">
         <v>401</v>
       </c>
@@ -24573,7 +24573,7 @@
       <c r="L472" s="97">
         <v>980</v>
       </c>
-      <c r="M472" s="210">
+      <c r="M472" s="208">
         <v>19</v>
       </c>
       <c r="N472" s="22">
@@ -24581,7 +24581,7 @@
         <v>52.833333333333336</v>
       </c>
     </row>
-    <row r="473" spans="1:15" s="28" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:15" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A473" s="49"/>
       <c r="B473" s="11" t="s">
         <v>43</v>
@@ -24620,7 +24620,7 @@
         <f t="shared" si="88"/>
         <v>7230</v>
       </c>
-      <c r="M473" s="211">
+      <c r="M473" s="209">
         <f t="shared" si="88"/>
         <v>71</v>
       </c>
@@ -24667,7 +24667,7 @@
       <c r="L474" s="97">
         <v>680</v>
       </c>
-      <c r="M474" s="210">
+      <c r="M474" s="208">
         <v>16</v>
       </c>
       <c r="N474" s="22">
@@ -24712,7 +24712,7 @@
       <c r="L475" s="97">
         <v>1040</v>
       </c>
-      <c r="M475" s="210">
+      <c r="M475" s="208">
         <v>22</v>
       </c>
       <c r="N475" s="22">
@@ -24757,7 +24757,7 @@
       <c r="L476" s="97">
         <v>450</v>
       </c>
-      <c r="M476" s="210">
+      <c r="M476" s="208">
         <v>12</v>
       </c>
       <c r="N476" s="22">
@@ -24804,7 +24804,7 @@
         <f t="shared" si="89"/>
         <v>2170</v>
       </c>
-      <c r="M477" s="211">
+      <c r="M477" s="209">
         <f t="shared" si="89"/>
         <v>50</v>
       </c>
@@ -24814,7 +24814,7 @@
       </c>
       <c r="O477" s="96"/>
     </row>
-    <row r="478" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A478" s="97">
         <v>405</v>
       </c>
@@ -24851,7 +24851,7 @@
       <c r="L478" s="97">
         <v>1100</v>
       </c>
-      <c r="M478" s="210">
+      <c r="M478" s="208">
         <v>24</v>
       </c>
       <c r="N478" s="22">
@@ -24859,7 +24859,7 @@
         <v>66.333333333333329</v>
       </c>
     </row>
-    <row r="479" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A479" s="97">
         <v>406</v>
       </c>
@@ -24896,7 +24896,7 @@
       <c r="L479" s="97">
         <v>760</v>
       </c>
-      <c r="M479" s="210">
+      <c r="M479" s="208">
         <v>12</v>
       </c>
       <c r="N479" s="22">
@@ -24904,7 +24904,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="480" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A480" s="97">
         <v>407</v>
       </c>
@@ -24941,7 +24941,7 @@
       <c r="L480" s="97">
         <v>900</v>
       </c>
-      <c r="M480" s="210">
+      <c r="M480" s="208">
         <v>10</v>
       </c>
       <c r="N480" s="22">
@@ -24949,7 +24949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="481" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A481" s="97">
         <v>408</v>
       </c>
@@ -24986,7 +24986,7 @@
       <c r="L481" s="97">
         <v>1010</v>
       </c>
-      <c r="M481" s="210">
+      <c r="M481" s="208">
         <v>10</v>
       </c>
       <c r="N481" s="22">
@@ -24994,7 +24994,7 @@
         <v>50.666666666666664</v>
       </c>
     </row>
-    <row r="482" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A482" s="97">
         <v>409</v>
       </c>
@@ -25031,7 +25031,7 @@
       <c r="L482" s="97">
         <v>770</v>
       </c>
-      <c r="M482" s="210">
+      <c r="M482" s="208">
         <v>1</v>
       </c>
       <c r="N482" s="22">
@@ -25039,7 +25039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="483" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A483" s="97">
         <v>410</v>
       </c>
@@ -25076,7 +25076,7 @@
       <c r="L483" s="97">
         <v>960</v>
       </c>
-      <c r="M483" s="210">
+      <c r="M483" s="208">
         <v>14</v>
       </c>
       <c r="N483" s="22">
@@ -25084,7 +25084,7 @@
         <v>63.166666666666664</v>
       </c>
     </row>
-    <row r="484" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A484" s="97">
         <v>411</v>
       </c>
@@ -25121,7 +25121,7 @@
       <c r="L484" s="97">
         <v>540</v>
       </c>
-      <c r="M484" s="210">
+      <c r="M484" s="208">
         <v>0</v>
       </c>
       <c r="N484" s="22">
@@ -25129,7 +25129,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="485" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A485" s="97">
         <v>412</v>
       </c>
@@ -25166,7 +25166,7 @@
       <c r="L485" s="97">
         <v>280</v>
       </c>
-      <c r="M485" s="210">
+      <c r="M485" s="208">
         <v>4</v>
       </c>
       <c r="N485" s="22">
@@ -25174,7 +25174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="486" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A486" s="97">
         <v>413</v>
       </c>
@@ -25211,7 +25211,7 @@
       <c r="L486" s="97">
         <v>180</v>
       </c>
-      <c r="M486" s="210">
+      <c r="M486" s="208">
         <v>0</v>
       </c>
       <c r="N486" s="22">
@@ -25219,7 +25219,7 @@
         <v>54.833333333333336</v>
       </c>
     </row>
-    <row r="487" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A487" s="97">
         <v>414</v>
       </c>
@@ -25256,7 +25256,7 @@
       <c r="L487" s="97">
         <v>310</v>
       </c>
-      <c r="M487" s="210">
+      <c r="M487" s="208">
         <v>2</v>
       </c>
       <c r="N487" s="22">
@@ -25264,7 +25264,7 @@
         <v>55.833333333333336</v>
       </c>
     </row>
-    <row r="488" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A488" s="97">
         <v>415</v>
       </c>
@@ -25301,7 +25301,7 @@
       <c r="L488" s="97">
         <v>290</v>
       </c>
-      <c r="M488" s="210">
+      <c r="M488" s="208">
         <v>3</v>
       </c>
       <c r="N488" s="22">
@@ -25309,7 +25309,7 @@
         <v>57.333333333333336</v>
       </c>
     </row>
-    <row r="489" spans="1:15" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:15" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A489" s="97">
         <v>416</v>
       </c>
@@ -25346,7 +25346,7 @@
       <c r="L489" s="97">
         <v>340</v>
       </c>
-      <c r="M489" s="210">
+      <c r="M489" s="208">
         <v>6</v>
       </c>
       <c r="N489" s="22">
@@ -25354,7 +25354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="490" spans="1:15" s="28" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:15" s="28" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A490" s="49"/>
       <c r="B490" s="11" t="s">
         <v>33</v>
@@ -25393,7 +25393,7 @@
         <f t="shared" si="91"/>
         <v>7440</v>
       </c>
-      <c r="M490" s="211">
+      <c r="M490" s="209">
         <f t="shared" si="91"/>
         <v>86</v>
       </c>
@@ -25440,7 +25440,7 @@
       <c r="L491" s="103">
         <v>1020</v>
       </c>
-      <c r="M491" s="212">
+      <c r="M491" s="210">
         <v>11</v>
       </c>
       <c r="N491" s="13">
@@ -25486,7 +25486,7 @@
       <c r="L492" s="103">
         <v>850</v>
       </c>
-      <c r="M492" s="212">
+      <c r="M492" s="210">
         <v>15</v>
       </c>
       <c r="N492" s="64">
@@ -25532,7 +25532,7 @@
       <c r="L493" s="103">
         <v>640</v>
       </c>
-      <c r="M493" s="212">
+      <c r="M493" s="210">
         <v>12</v>
       </c>
       <c r="N493" s="84">
@@ -25577,7 +25577,7 @@
       <c r="L494" s="103">
         <v>900</v>
       </c>
-      <c r="M494" s="212">
+      <c r="M494" s="210">
         <v>8</v>
       </c>
       <c r="N494" s="84">
@@ -25622,7 +25622,7 @@
       <c r="L495" s="103">
         <v>750</v>
       </c>
-      <c r="M495" s="212">
+      <c r="M495" s="210">
         <v>19</v>
       </c>
       <c r="N495" s="84">
@@ -25667,7 +25667,7 @@
       <c r="L496" s="103">
         <v>360</v>
       </c>
-      <c r="M496" s="212">
+      <c r="M496" s="210">
         <v>12</v>
       </c>
       <c r="N496" s="84">
@@ -25712,7 +25712,7 @@
       <c r="L497" s="103">
         <v>480</v>
       </c>
-      <c r="M497" s="212">
+      <c r="M497" s="210">
         <v>10</v>
       </c>
       <c r="N497" s="84">
@@ -25759,7 +25759,7 @@
         <f t="shared" si="93"/>
         <v>5000</v>
       </c>
-      <c r="M498" s="213">
+      <c r="M498" s="211">
         <f t="shared" si="93"/>
         <v>87</v>
       </c>
@@ -25806,7 +25806,7 @@
       <c r="L499" s="103">
         <v>400</v>
       </c>
-      <c r="M499" s="212">
+      <c r="M499" s="210">
         <v>24</v>
       </c>
       <c r="N499" s="84">
@@ -25851,7 +25851,7 @@
       <c r="L500" s="136">
         <v>1100</v>
       </c>
-      <c r="M500" s="214">
+      <c r="M500" s="212">
         <v>16</v>
       </c>
       <c r="N500" s="171">
@@ -25897,7 +25897,7 @@
       <c r="L501" s="136">
         <v>740</v>
       </c>
-      <c r="M501" s="214">
+      <c r="M501" s="212">
         <v>9</v>
       </c>
       <c r="N501" s="171">
@@ -25943,7 +25943,7 @@
       <c r="L502" s="136">
         <v>760</v>
       </c>
-      <c r="M502" s="214">
+      <c r="M502" s="212">
         <v>10</v>
       </c>
       <c r="N502" s="171">
@@ -25989,7 +25989,7 @@
       <c r="L503" s="136">
         <v>680</v>
       </c>
-      <c r="M503" s="214">
+      <c r="M503" s="212">
         <v>16</v>
       </c>
       <c r="N503" s="171">
@@ -26037,7 +26037,7 @@
         <f t="shared" si="94"/>
         <v>3680</v>
       </c>
-      <c r="M504" s="215">
+      <c r="M504" s="213">
         <f t="shared" si="94"/>
         <v>75</v>
       </c>
@@ -26084,7 +26084,7 @@
       <c r="L505" s="136">
         <v>800</v>
       </c>
-      <c r="M505" s="214">
+      <c r="M505" s="212">
         <v>12</v>
       </c>
       <c r="N505" s="171">
@@ -26130,7 +26130,7 @@
       <c r="L506" s="136">
         <v>650</v>
       </c>
-      <c r="M506" s="214">
+      <c r="M506" s="212">
         <v>20</v>
       </c>
       <c r="N506" s="171">
@@ -26176,7 +26176,7 @@
       <c r="L507" s="136">
         <v>640</v>
       </c>
-      <c r="M507" s="214">
+      <c r="M507" s="212">
         <v>18</v>
       </c>
       <c r="N507" s="171">
@@ -26224,7 +26224,7 @@
         <f t="shared" si="95"/>
         <v>2090</v>
       </c>
-      <c r="M508" s="215">
+      <c r="M508" s="213">
         <f t="shared" si="95"/>
         <v>50</v>
       </c>
@@ -26271,7 +26271,7 @@
       <c r="L509" s="136">
         <v>1050</v>
       </c>
-      <c r="M509" s="214">
+      <c r="M509" s="212">
         <v>21</v>
       </c>
       <c r="N509" s="171">
@@ -26317,7 +26317,7 @@
       <c r="L510" s="136">
         <v>900</v>
       </c>
-      <c r="M510" s="214">
+      <c r="M510" s="212">
         <v>24</v>
       </c>
       <c r="N510" s="171">
@@ -26363,7 +26363,7 @@
       <c r="L511" s="136">
         <v>880</v>
       </c>
-      <c r="M511" s="214">
+      <c r="M511" s="212">
         <v>14</v>
       </c>
       <c r="N511" s="171">
@@ -26409,7 +26409,7 @@
       <c r="L512" s="136">
         <v>480</v>
       </c>
-      <c r="M512" s="214">
+      <c r="M512" s="212">
         <v>8</v>
       </c>
       <c r="N512" s="171">
@@ -26457,7 +26457,7 @@
         <f t="shared" si="96"/>
         <v>3310</v>
       </c>
-      <c r="M513" s="215">
+      <c r="M513" s="213">
         <f t="shared" si="96"/>
         <v>67</v>
       </c>
@@ -26504,7 +26504,7 @@
       <c r="L514" s="136">
         <v>720</v>
       </c>
-      <c r="M514" s="214">
+      <c r="M514" s="212">
         <v>11</v>
       </c>
       <c r="N514" s="171">
@@ -26550,7 +26550,7 @@
       <c r="L515" s="136">
         <v>640</v>
       </c>
-      <c r="M515" s="214">
+      <c r="M515" s="212">
         <v>8</v>
       </c>
       <c r="N515" s="171">
@@ -26596,7 +26596,7 @@
       <c r="L516" s="136">
         <v>480</v>
       </c>
-      <c r="M516" s="214">
+      <c r="M516" s="212">
         <v>9</v>
       </c>
       <c r="N516" s="171">
@@ -26644,7 +26644,7 @@
         <f t="shared" si="97"/>
         <v>1840</v>
       </c>
-      <c r="M517" s="215">
+      <c r="M517" s="213">
         <f t="shared" si="97"/>
         <v>28</v>
       </c>
@@ -26691,7 +26691,7 @@
       <c r="L518" s="176">
         <v>840</v>
       </c>
-      <c r="M518" s="216">
+      <c r="M518" s="214">
         <v>14</v>
       </c>
       <c r="N518" s="178">
@@ -26737,7 +26737,7 @@
       <c r="L519" s="176">
         <v>480</v>
       </c>
-      <c r="M519" s="216">
+      <c r="M519" s="214">
         <v>21</v>
       </c>
       <c r="N519" s="178">
@@ -26783,7 +26783,7 @@
       <c r="L520" s="176">
         <v>380</v>
       </c>
-      <c r="M520" s="216">
+      <c r="M520" s="214">
         <v>18</v>
       </c>
       <c r="N520" s="178">
@@ -26829,7 +26829,7 @@
       <c r="L521" s="176">
         <v>540</v>
       </c>
-      <c r="M521" s="216">
+      <c r="M521" s="214">
         <v>12</v>
       </c>
       <c r="N521" s="178">
@@ -26875,7 +26875,7 @@
       <c r="L522" s="176">
         <v>640</v>
       </c>
-      <c r="M522" s="216">
+      <c r="M522" s="214">
         <v>16</v>
       </c>
       <c r="N522" s="178">
@@ -26921,7 +26921,7 @@
       <c r="L523" s="176">
         <v>480</v>
       </c>
-      <c r="M523" s="216">
+      <c r="M523" s="214">
         <v>21</v>
       </c>
       <c r="N523" s="178">
@@ -26967,7 +26967,7 @@
       <c r="L524" s="176">
         <v>400</v>
       </c>
-      <c r="M524" s="216">
+      <c r="M524" s="214">
         <v>10</v>
       </c>
       <c r="N524" s="178">
@@ -27013,7 +27013,7 @@
       <c r="L525" s="176">
         <v>640</v>
       </c>
-      <c r="M525" s="216">
+      <c r="M525" s="214">
         <v>14</v>
       </c>
       <c r="N525" s="178">
@@ -27059,7 +27059,7 @@
       <c r="L526" s="176">
         <v>360</v>
       </c>
-      <c r="M526" s="216">
+      <c r="M526" s="214">
         <v>20</v>
       </c>
       <c r="N526" s="178">
@@ -27105,7 +27105,7 @@
       <c r="L527" s="176">
         <v>480</v>
       </c>
-      <c r="M527" s="216">
+      <c r="M527" s="214">
         <v>8</v>
       </c>
       <c r="N527" s="178">
@@ -27151,7 +27151,7 @@
       <c r="L528" s="176">
         <v>450</v>
       </c>
-      <c r="M528" s="216">
+      <c r="M528" s="214">
         <v>28</v>
       </c>
       <c r="N528" s="178">
@@ -27197,7 +27197,7 @@
       <c r="L529" s="176">
         <v>720</v>
       </c>
-      <c r="M529" s="216">
+      <c r="M529" s="214">
         <v>0</v>
       </c>
       <c r="N529" s="178">
@@ -27243,7 +27243,7 @@
       <c r="L530" s="176">
         <v>280</v>
       </c>
-      <c r="M530" s="216">
+      <c r="M530" s="214">
         <v>14</v>
       </c>
       <c r="N530" s="178">
@@ -27289,7 +27289,7 @@
       <c r="L531" s="176">
         <v>360</v>
       </c>
-      <c r="M531" s="216">
+      <c r="M531" s="214">
         <v>15</v>
       </c>
       <c r="N531" s="178">
@@ -27337,7 +27337,7 @@
         <f t="shared" si="99"/>
         <v>7050</v>
       </c>
-      <c r="M532" s="217">
+      <c r="M532" s="215">
         <f t="shared" si="99"/>
         <v>211</v>
       </c>
@@ -27384,7 +27384,7 @@
       <c r="L533" s="109">
         <v>540</v>
       </c>
-      <c r="M533" s="218">
+      <c r="M533" s="216">
         <v>12</v>
       </c>
       <c r="N533" s="182">
@@ -27432,7 +27432,7 @@
         <f t="shared" si="100"/>
         <v>540</v>
       </c>
-      <c r="M534" s="217">
+      <c r="M534" s="215">
         <f t="shared" si="100"/>
         <v>12</v>
       </c>
@@ -27481,7 +27481,7 @@
         <f>SUBTOTAL(9, L4:L534)</f>
         <v>704792</v>
       </c>
-      <c r="M535" s="219">
+      <c r="M535" s="217">
         <f>SUBTOTAL(9, M4:M534)</f>
         <v>5315.4</v>
       </c>
@@ -27504,7 +27504,7 @@
       <c r="J536" s="109"/>
       <c r="K536" s="109"/>
       <c r="L536" s="109"/>
-      <c r="M536" s="218"/>
+      <c r="M536" s="216"/>
       <c r="N536" s="162"/>
       <c r="O536" s="162"/>
     </row>
@@ -27666,21 +27666,7 @@
       <c r="O547" s="162"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O294" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0" showButton="0"/>
-    <filterColumn colId="1" showButton="0"/>
-    <filterColumn colId="2" showButton="0"/>
-    <filterColumn colId="3" showButton="0"/>
-    <filterColumn colId="4" showButton="0"/>
-    <filterColumn colId="5" showButton="0"/>
-    <filterColumn colId="6" showButton="0"/>
-    <filterColumn colId="7" showButton="0"/>
-    <filterColumn colId="8" showButton="0"/>
-    <filterColumn colId="9" showButton="0"/>
-    <filterColumn colId="10" showButton="0"/>
-    <filterColumn colId="11" showButton="0"/>
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
+  <autoFilter ref="A2:O534" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:DL370">
     <sortCondition ref="D3:D370"/>
   </sortState>
@@ -28014,20 +28000,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="145" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="203"/>
-      <c r="B1" s="203"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="203"/>
-      <c r="E1" s="203"/>
-      <c r="F1" s="203"/>
-      <c r="G1" s="203"/>
-      <c r="H1" s="203"/>
-      <c r="I1" s="203"/>
-      <c r="J1" s="203"/>
-      <c r="K1" s="203"/>
-      <c r="L1" s="203"/>
-      <c r="M1" s="203"/>
-      <c r="N1" s="203"/>
+      <c r="A1" s="218"/>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+      <c r="K1" s="218"/>
+      <c r="L1" s="218"/>
+      <c r="M1" s="218"/>
+      <c r="N1" s="218"/>
     </row>
     <row r="2" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
@@ -33692,20 +33678,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="161" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="204"/>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="204"/>
-      <c r="N1" s="204"/>
+      <c r="A1" s="219"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
+      <c r="H1" s="219"/>
+      <c r="I1" s="219"/>
+      <c r="J1" s="219"/>
+      <c r="K1" s="219"/>
+      <c r="L1" s="219"/>
+      <c r="M1" s="219"/>
+      <c r="N1" s="219"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="110" t="s">

</xml_diff>